<commit_message>
updated the BOM by highlighting the components we have in stock
</commit_message>
<xml_diff>
--- a/Hardware/Design Files/Light Module/Light_Module_BOM.xlsx
+++ b/Hardware/Design Files/Light Module/Light_Module_BOM.xlsx
@@ -508,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -516,9 +516,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -598,7 +595,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,6 +632,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,11 +654,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Teensy_Board" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_module_BOM" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tentacle_module_BOM" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Teensy_Board" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -932,7 +931,7 @@
   <dimension ref="A2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1772,573 +1771,573 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-    </row>
-    <row r="5" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+    </row>
+    <row r="5" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="33"/>
-    </row>
-    <row r="6" spans="1:13" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
-        <v>1</v>
-      </c>
-      <c r="B6" s="29" t="s">
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="32"/>
+    </row>
+    <row r="6" spans="1:13" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>1</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="30">
-        <v>1</v>
-      </c>
-      <c r="E6" s="23" t="s">
+      <c r="D6" s="29">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24" t="s">
+      <c r="G6" s="22"/>
+      <c r="H6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-    </row>
-    <row r="7" spans="1:13" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
+      <c r="I6" s="23"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
         <v>2</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="30">
-        <v>1</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="29">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-    </row>
-    <row r="8" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="40">
+      <c r="I7" s="20"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
         <v>3</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="50">
-        <v>1</v>
-      </c>
-      <c r="E8" s="44" t="s">
+      <c r="D8" s="48">
+        <v>1</v>
+      </c>
+      <c r="E8" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="50">
         <v>1206</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="53"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-    </row>
-    <row r="9" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="50">
+      <c r="I8" s="51"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+    </row>
+    <row r="9" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="48">
         <v>4</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="43">
-        <v>1</v>
-      </c>
-      <c r="E9" s="52" t="s">
+      <c r="D9" s="41">
+        <v>1</v>
+      </c>
+      <c r="E9" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="53"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-    </row>
-    <row r="10" spans="1:13" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="I9" s="51"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+    </row>
+    <row r="10" spans="1:13" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
         <v>5</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="35">
-        <v>1</v>
-      </c>
-      <c r="E10" s="36" t="s">
+      <c r="D10" s="34">
+        <v>1</v>
+      </c>
+      <c r="E10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-    </row>
-    <row r="11" spans="1:13" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
+      <c r="I10" s="23"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+    </row>
+    <row r="11" spans="1:13" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
         <v>6</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="30">
-        <v>1</v>
-      </c>
-      <c r="E11" s="26" t="s">
+      <c r="D11" s="29">
+        <v>1</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-    </row>
-    <row r="12" spans="1:13" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="I11" s="23"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
         <v>7</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <v>2</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-    </row>
-    <row r="13" spans="1:13" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="25">
+      <c r="I12" s="23"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+    </row>
+    <row r="13" spans="1:13" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
         <v>8</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="30">
-        <v>1</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="29">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-    </row>
-    <row r="14" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="40">
+      <c r="I13" s="20"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+    </row>
+    <row r="14" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
         <v>9</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="41">
         <v>2</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="47"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-    </row>
-    <row r="15" spans="1:13" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+      <c r="I14" s="45"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+    </row>
+    <row r="15" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="48">
         <v>10</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="20">
-        <v>1</v>
-      </c>
-      <c r="E15" s="21" t="s">
+      <c r="D15" s="48">
+        <v>1</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-    </row>
-    <row r="16" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="40">
+      <c r="I15" s="45"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+    </row>
+    <row r="16" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
         <v>11</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="50">
-        <v>1</v>
-      </c>
-      <c r="E16" s="44" t="s">
+      <c r="D16" s="48">
+        <v>1</v>
+      </c>
+      <c r="E16" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-    </row>
-    <row r="17" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="40">
+      <c r="I16" s="45"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+    </row>
+    <row r="17" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
         <v>12</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="50">
-        <v>1</v>
-      </c>
-      <c r="E17" s="44" t="s">
+      <c r="D17" s="48">
+        <v>1</v>
+      </c>
+      <c r="E17" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="46" t="s">
+      <c r="H17" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="47"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-    </row>
-    <row r="18" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="50">
+      <c r="I17" s="45"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+    </row>
+    <row r="18" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="48">
         <v>13</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="43">
-        <v>1</v>
-      </c>
-      <c r="E18" s="47" t="s">
+      <c r="D18" s="41">
+        <v>1</v>
+      </c>
+      <c r="E18" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="46" t="s">
+      <c r="G18" s="42"/>
+      <c r="H18" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="47"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-    </row>
-    <row r="19" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="40">
+      <c r="I18" s="45"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+    </row>
+    <row r="19" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
         <v>14</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="56">
-        <v>1</v>
-      </c>
-      <c r="E19" s="57" t="s">
+      <c r="D19" s="54">
+        <v>1</v>
+      </c>
+      <c r="E19" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="59" t="s">
+      <c r="H19" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-    </row>
-    <row r="20" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="40">
+      <c r="I19" s="45"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+    </row>
+    <row r="20" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
         <v>15</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="56">
-        <v>1</v>
-      </c>
-      <c r="E20" s="59" t="s">
+      <c r="D20" s="54">
+        <v>1</v>
+      </c>
+      <c r="E20" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="G20" s="57"/>
-      <c r="H20" s="59" t="s">
+      <c r="G20" s="55"/>
+      <c r="H20" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="47"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-    </row>
-    <row r="21" spans="1:13" s="48" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="50">
+      <c r="I20" s="45"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+    </row>
+    <row r="21" spans="1:13" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="48">
         <v>16</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="56">
-        <v>1</v>
-      </c>
-      <c r="E21" s="59" t="s">
+      <c r="D21" s="54">
+        <v>1</v>
+      </c>
+      <c r="E21" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="57" t="s">
+      <c r="G21" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="59" t="s">
+      <c r="H21" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="46"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-    </row>
-    <row r="22" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="G22" s="28"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-    </row>
-    <row r="23" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="G23" s="28"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-    </row>
-    <row r="24" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="G24" s="28"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
+      <c r="I21" s="44"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+    </row>
+    <row r="22" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="G22" s="27"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+    </row>
+    <row r="23" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="G23" s="27"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+    </row>
+    <row r="24" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="G24" s="27"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2364,7 +2363,7 @@
     <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="46.7109375" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2376,62 +2375,62 @@
       <c r="A1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="9"/>
+      <c r="E1" s="8"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="9"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2445,7 +2444,7 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>1</v>
       </c>
       <c r="F6" t="s">
@@ -2462,7 +2461,7 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>1</v>
       </c>
       <c r="F7" t="s">
@@ -2479,7 +2478,7 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>1</v>
       </c>
       <c r="F8" t="s">
@@ -2496,7 +2495,7 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>1</v>
       </c>
       <c r="F9" t="s">
@@ -2513,7 +2512,7 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>1</v>
       </c>
       <c r="F10" t="s">
@@ -2530,7 +2529,7 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
@@ -2547,7 +2546,7 @@
       <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>1</v>
       </c>
       <c r="F12" t="s">
@@ -2564,7 +2563,7 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>1</v>
       </c>
       <c r="F13" t="s">
@@ -2584,7 +2583,7 @@
       <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>2</v>
       </c>
       <c r="F14" t="s">
@@ -2604,7 +2603,7 @@
       <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>1</v>
       </c>
       <c r="F15" t="s">
@@ -2624,7 +2623,7 @@
       <c r="D16">
         <v>470</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>1</v>
       </c>
       <c r="F16" t="s">
@@ -2644,7 +2643,7 @@
       <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>1</v>
       </c>
       <c r="F17" t="s">
@@ -2661,7 +2660,7 @@
       <c r="D18">
         <v>5.6</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <v>1</v>
       </c>
       <c r="F18" t="s">
@@ -2681,7 +2680,7 @@
       <c r="D19" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="11">
         <v>1</v>
       </c>
       <c r="F19" t="s">
@@ -2701,7 +2700,7 @@
       <c r="D20" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="11">
         <v>1</v>
       </c>
       <c r="F20" t="s">
@@ -2721,7 +2720,7 @@
       <c r="D21" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="11">
         <v>1</v>
       </c>
       <c r="F21" t="s">

</xml_diff>